<commit_message>
add other test for 0.61
</commit_message>
<xml_diff>
--- a/test/perl_output/merge4.xlsx
+++ b/test/perl_output/merge4.xlsx
@@ -413,7 +413,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" ht="30" customHeight="1"/>
+    <row r="4" spans="2:4" ht="30" customHeight="1"/>
     <row r="5" spans="2:4" ht="30" customHeight="1">
       <c r="B5" s="2" t="s">
         <v>1</v>
@@ -426,7 +426,7 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" ht="30" customHeight="1"/>
+    <row r="7" spans="2:4" ht="30" customHeight="1"/>
     <row r="8" spans="2:4" ht="30" customHeight="1">
       <c r="B8" s="3" t="s">
         <v>2</v>
@@ -439,7 +439,7 @@
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" ht="30" customHeight="1"/>
+    <row r="10" spans="2:4" ht="30" customHeight="1"/>
     <row r="11" spans="2:4" ht="30" customHeight="1">
       <c r="B11" s="4" t="s">
         <v>3</v>

</xml_diff>